<commit_message>
fixed buf of campaign filter
</commit_message>
<xml_diff>
--- a/insight/report.xlsx
+++ b/insight/report.xlsx
@@ -72,13 +72,13 @@
     <t>Video</t>
   </si>
   <si>
-    <t>Vivek</t>
+    <t>Campaign1</t>
   </si>
   <si>
     <t>Photo</t>
   </si>
   <si>
-    <t>Bhavesh</t>
+    <t>Campaign2</t>
   </si>
 </sst>
 </file>

</xml_diff>